<commit_message>
versão do site do fse ao enviar a versão final
</commit_message>
<xml_diff>
--- a/fse-2017-data/download/non-removal-patterns.xlsx
+++ b/fse-2017-data/download/non-removal-patterns.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Sites/diegocedrim.github.io/icse-2017-data/download/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Sites/diegocedrim.github.io/fse-2017-data/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="29">
   <si>
     <t>ref_name</t>
   </si>
@@ -484,7 +484,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,76 +893,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2">
-        <v>666</v>
-      </c>
-      <c r="D20" s="2">
-        <v>11017</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>6.0452028682944539E-2</v>
-      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1256</v>
-      </c>
-      <c r="D21" s="2">
-        <v>11017</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.11400562766633385</v>
-      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2">
-        <v>56</v>
-      </c>
-      <c r="D22" s="2">
-        <v>11017</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="0"/>
-        <v>5.0830534628301715E-3</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="2">
-        <v>382</v>
-      </c>
-      <c r="D23" s="2">
-        <v>11017</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4673686121448673E-2</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>